<commit_message>
Task 1 some changes
</commit_message>
<xml_diff>
--- a/Final task/Final Task - Data Testing approaches/Flights_Check_List_Anastasiya_Viktarovich.xlsx
+++ b/Final task/Final Task - Data Testing approaches/Flights_Check_List_Anastasiya_Viktarovich.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anastasiya_Viktarovi\Documents\GitHub\Data-Quality-Engineering-Mentoring-Program-Intermediate-Level-9\Final task\Final Task - Data Testing approaches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69257BD6-8311-4BB8-8ED8-8C46404C114D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD5B38A-B220-4C0E-A2E8-CAE136D78DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="63">
   <si>
     <t>Table</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Validity</t>
-  </si>
-  <si>
-    <t>All tables have required column names</t>
   </si>
   <si>
     <t>Carriers</t>
@@ -261,7 +258,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -284,24 +281,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF70DAE2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF70DAE2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF70DAE2"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -321,24 +305,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,8 +458,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4832A521-5338-49CC-B06C-CE36D0D010CD}" name="Table1" displayName="Table1" ref="A1:E35" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E35" xr:uid="{7B8C9D4B-D90E-4FA4-B19D-E5C3195B7DC2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4832A521-5338-49CC-B06C-CE36D0D010CD}" name="Table1" displayName="Table1" ref="A1:E34" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A1:E34" xr:uid="{7B8C9D4B-D90E-4FA4-B19D-E5C3195B7DC2}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{A172624E-2B65-4767-91E6-0D25BD5BC644}" name="#" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{6ADFB97F-321E-45E8-8276-C3A592BA3E0A}" name="Table" dataDxfId="3"/>
@@ -768,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -831,7 +797,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
@@ -842,13 +808,13 @@
         <v>5</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
@@ -856,16 +822,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
@@ -873,16 +839,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
@@ -890,16 +856,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>15</v>
+      <c r="E7" s="5" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
@@ -907,16 +873,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
@@ -924,13 +890,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>17</v>
@@ -941,16 +907,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
@@ -958,16 +924,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>12</v>
+      <c r="E11" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
@@ -975,15 +941,15 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>21</v>
       </c>
     </row>
@@ -992,16 +958,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>5</v>
-      </c>
       <c r="E13" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
@@ -1009,13 +975,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>24</v>
@@ -1026,16 +992,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
@@ -1043,13 +1009,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>59</v>
@@ -1060,16 +1026,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
@@ -1077,16 +1043,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
@@ -1094,16 +1060,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
@@ -1111,7 +1077,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>9</v>
@@ -1120,7 +1086,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
@@ -1128,16 +1094,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
@@ -1145,16 +1111,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
@@ -1162,16 +1128,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
@@ -1179,16 +1145,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
@@ -1196,16 +1162,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>63</v>
+      <c r="E25" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
@@ -1213,169 +1179,152 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E26" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>26</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E27" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E29" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E29" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <v>29</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>48</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
         <v>30</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D31" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>31</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E32" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
         <v>32</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E33" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="7" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
         <v>33</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="4">
-        <v>34</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Task 2 some changes
</commit_message>
<xml_diff>
--- a/Final task/Final Task - Data Testing approaches/Flights_Check_List_Anastasiya_Viktarovich.xlsx
+++ b/Final task/Final Task - Data Testing approaches/Flights_Check_List_Anastasiya_Viktarovich.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anastasiya_Viktarovi\Documents\GitHub\Data-Quality-Engineering-Mentoring-Program-Intermediate-Level-9\Final task\Final Task - Data Testing approaches\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD5B38A-B220-4C0E-A2E8-CAE136D78DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4DEF4D-3203-4179-B1E0-5C84103AB249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -737,7 +737,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>